<commit_message>
test all the import service
</commit_message>
<xml_diff>
--- a/data/score_list.xlsx
+++ b/data/score_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huangjiani/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huangjiani/CourseSelectionSystem/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A92A1A-32A1-0848-BB46-A632BA9B66B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE240118-E8B3-D84E-826B-16B133CB0ED1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8680" yWindow="880" windowWidth="27640" windowHeight="15920" xr2:uid="{F568A169-15F7-3C46-A23E-EBAF81D00A1A}"/>
+    <workbookView xWindow="13560" yWindow="1980" windowWidth="27640" windowHeight="15920" xr2:uid="{F568A169-15F7-3C46-A23E-EBAF81D00A1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>course_id</t>
   </si>
@@ -43,6 +43,24 @@
   </si>
   <si>
     <t>score</t>
+  </si>
+  <si>
+    <t>SOFT130015</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>BIOL110007</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>SOFT130049</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -394,13 +412,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A12A9F42-956A-4748-96C3-833ED4BBD63C}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -414,6 +435,48 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>17302010049</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>17302010049</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>17302010049</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>